<commit_message>
#ExcelTest : .java file reader complete
ToDo: Fix .exe error
</commit_message>
<xml_diff>
--- a/FMS.xlsx
+++ b/FMS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3747" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3747" uniqueCount="454">
   <si>
     <t>FMS Table Definition</t>
   </si>
@@ -582,9 +582,6 @@
   </si>
   <si>
     <t xml:space="preserve"> photoUrl</t>
-  </si>
-  <si>
-    <t>,value=</t>
   </si>
   <si>
     <t xml:space="preserve"> type</t>
@@ -6257,7 +6254,7 @@
         <v>189</v>
       </c>
       <c r="D174" s="63" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="E174" s="63" t="s">
         <v>22</v>
@@ -6278,7 +6275,7 @@
     </row>
     <row r="175">
       <c r="C175" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D175" s="63" t="s">
         <v>19</v>
@@ -6392,13 +6389,13 @@
         <v>80</v>
       </c>
       <c r="B180" s="70" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C180" s="69" t="s">
         <v>14</v>
       </c>
       <c r="D180" s="69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E180" s="69" t="s">
         <v>16</v>
@@ -6446,7 +6443,7 @@
         <v>86</v>
       </c>
       <c r="D182" s="69" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E182" s="69" t="s">
         <v>16</v>
@@ -6494,7 +6491,7 @@
         <v>91</v>
       </c>
       <c r="D184" s="69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E184" s="69" t="s">
         <v>22</v>
@@ -6518,7 +6515,7 @@
         <v>87</v>
       </c>
       <c r="D185" s="69" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E185" s="69" t="s">
         <v>22</v>
@@ -6542,7 +6539,7 @@
         <v>89</v>
       </c>
       <c r="D186" s="69" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E186" s="69" t="s">
         <v>22</v>
@@ -6563,10 +6560,10 @@
     </row>
     <row r="187">
       <c r="C187" s="69" t="s">
+        <v>197</v>
+      </c>
+      <c r="D187" s="69" t="s">
         <v>198</v>
-      </c>
-      <c r="D187" s="69" t="s">
-        <v>199</v>
       </c>
       <c r="E187" s="69" t="s">
         <v>22</v>
@@ -6590,7 +6587,7 @@
         <v>115</v>
       </c>
       <c r="D188" s="69" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E188" s="69" t="s">
         <v>22</v>
@@ -6611,10 +6608,10 @@
     </row>
     <row r="189">
       <c r="C189" s="69" t="s">
+        <v>200</v>
+      </c>
+      <c r="D189" s="69" t="s">
         <v>201</v>
-      </c>
-      <c r="D189" s="69" t="s">
-        <v>202</v>
       </c>
       <c r="E189" s="69" t="s">
         <v>22</v>
@@ -6635,10 +6632,10 @@
     </row>
     <row r="190">
       <c r="C190" s="69" t="s">
+        <v>202</v>
+      </c>
+      <c r="D190" s="69" t="s">
         <v>203</v>
-      </c>
-      <c r="D190" s="69" t="s">
-        <v>204</v>
       </c>
       <c r="E190" s="69" t="s">
         <v>22</v>
@@ -6659,10 +6656,10 @@
     </row>
     <row r="191">
       <c r="C191" s="69" t="s">
+        <v>204</v>
+      </c>
+      <c r="D191" s="69" t="s">
         <v>205</v>
-      </c>
-      <c r="D191" s="69" t="s">
-        <v>206</v>
       </c>
       <c r="E191" s="69" t="s">
         <v>22</v>
@@ -6685,10 +6682,10 @@
       <c r="A192" s="70"/>
       <c r="B192" s="70"/>
       <c r="C192" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="D192" s="70" t="s">
         <v>207</v>
-      </c>
-      <c r="D192" s="70" t="s">
-        <v>208</v>
       </c>
       <c r="E192" s="70" t="s">
         <v>22</v>
@@ -6746,16 +6743,16 @@
     </row>
     <row r="195">
       <c r="A195" s="76" t="s">
+        <v>208</v>
+      </c>
+      <c r="B195" s="76" t="s">
         <v>209</v>
-      </c>
-      <c r="B195" s="76" t="s">
-        <v>210</v>
       </c>
       <c r="C195" s="75" t="s">
         <v>14</v>
       </c>
       <c r="D195" s="75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E195" s="75" t="s">
         <v>16</v>
@@ -6776,10 +6773,10 @@
     </row>
     <row r="196">
       <c r="C196" s="75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D196" s="75" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E196" s="75" t="s">
         <v>16</v>
@@ -6800,19 +6797,19 @@
     </row>
     <row r="197">
       <c r="C197" s="75" t="s">
+        <v>212</v>
+      </c>
+      <c r="D197" s="75" t="s">
         <v>213</v>
       </c>
-      <c r="D197" s="75" t="s">
+      <c r="E197" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="F197" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="G197" s="75" t="s">
         <v>214</v>
-      </c>
-      <c r="E197" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="F197" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="G197" s="75" t="s">
-        <v>215</v>
       </c>
       <c r="H197" s="75" t="s">
         <v>19</v>
@@ -6824,10 +6821,10 @@
     </row>
     <row r="198">
       <c r="C198" s="75" t="s">
+        <v>215</v>
+      </c>
+      <c r="D198" s="75" t="s">
         <v>216</v>
-      </c>
-      <c r="D198" s="75" t="s">
-        <v>217</v>
       </c>
       <c r="E198" s="75" t="s">
         <v>22</v>
@@ -6848,19 +6845,19 @@
     </row>
     <row r="199">
       <c r="C199" s="75" t="s">
+        <v>217</v>
+      </c>
+      <c r="D199" s="75" t="s">
         <v>218</v>
       </c>
-      <c r="D199" s="75" t="s">
+      <c r="E199" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="F199" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="G199" s="75" t="s">
         <v>219</v>
-      </c>
-      <c r="E199" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="F199" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="G199" s="75" t="s">
-        <v>220</v>
       </c>
       <c r="H199" s="75" t="s">
         <v>19</v>
@@ -6872,11 +6869,11 @@
     </row>
     <row r="200">
       <c r="C200" s="75" t="s">
+        <v>220</v>
+      </c>
+      <c r="D200" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="D200" s="75" t="s">
-        <v>222</v>
-      </c>
       <c r="E200" s="75" t="s">
         <v>22</v>
       </c>
@@ -6884,7 +6881,7 @@
         <v>17</v>
       </c>
       <c r="G200" s="75" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H200" s="75" t="s">
         <v>19</v>
@@ -6898,10 +6895,10 @@
       <c r="A201" s="76"/>
       <c r="B201" s="76"/>
       <c r="C201" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="D201" s="76" t="s">
         <v>223</v>
-      </c>
-      <c r="D201" s="76" t="s">
-        <v>224</v>
       </c>
       <c r="E201" s="76" t="s">
         <v>22</v>
@@ -6959,16 +6956,16 @@
     </row>
     <row r="204">
       <c r="A204" s="82" t="s">
+        <v>224</v>
+      </c>
+      <c r="B204" s="82" t="s">
         <v>225</v>
-      </c>
-      <c r="B204" s="82" t="s">
-        <v>226</v>
       </c>
       <c r="C204" s="81" t="s">
         <v>14</v>
       </c>
       <c r="D204" s="81" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E204" s="81" t="s">
         <v>16</v>
@@ -6989,10 +6986,10 @@
     </row>
     <row r="205">
       <c r="C205" s="81" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D205" s="81" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E205" s="81" t="s">
         <v>16</v>
@@ -7013,10 +7010,10 @@
     </row>
     <row r="206">
       <c r="C206" s="81" t="s">
+        <v>204</v>
+      </c>
+      <c r="D206" s="81" t="s">
         <v>205</v>
-      </c>
-      <c r="D206" s="81" t="s">
-        <v>206</v>
       </c>
       <c r="E206" s="81" t="s">
         <v>22</v>
@@ -7039,16 +7036,16 @@
       <c r="A207" s="82"/>
       <c r="B207" s="82"/>
       <c r="C207" s="82" t="s">
+        <v>227</v>
+      </c>
+      <c r="D207" s="82" t="s">
         <v>228</v>
       </c>
-      <c r="D207" s="82" t="s">
-        <v>229</v>
-      </c>
       <c r="E207" s="82" t="s">
         <v>22</v>
       </c>
       <c r="F207" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G207" s="82" t="s">
         <v>19</v>
@@ -7100,16 +7097,16 @@
     </row>
     <row r="210">
       <c r="A210" s="88" t="s">
+        <v>229</v>
+      </c>
+      <c r="B210" s="88" t="s">
         <v>230</v>
-      </c>
-      <c r="B210" s="88" t="s">
-        <v>231</v>
       </c>
       <c r="C210" s="87" t="s">
         <v>14</v>
       </c>
       <c r="D210" s="87" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E210" s="87" t="s">
         <v>16</v>
@@ -7130,10 +7127,10 @@
     </row>
     <row r="211">
       <c r="C211" s="87" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D211" s="87" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E211" s="87" t="s">
         <v>16</v>
@@ -7157,7 +7154,7 @@
         <v>115</v>
       </c>
       <c r="D212" s="87" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E212" s="87" t="s">
         <v>22</v>
@@ -7181,7 +7178,7 @@
         <v>118</v>
       </c>
       <c r="D213" s="87" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E213" s="87" t="s">
         <v>16</v>
@@ -7204,10 +7201,10 @@
       <c r="A214" s="88"/>
       <c r="B214" s="88"/>
       <c r="C214" s="88" t="s">
+        <v>233</v>
+      </c>
+      <c r="D214" s="88" t="s">
         <v>234</v>
-      </c>
-      <c r="D214" s="88" t="s">
-        <v>235</v>
       </c>
       <c r="E214" s="88" t="s">
         <v>22</v>
@@ -7415,7 +7412,7 @@
     </row>
     <row r="223">
       <c r="C223" s="93" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D223" s="93" t="s">
         <v>19</v>
@@ -7439,7 +7436,7 @@
     </row>
     <row r="224">
       <c r="C224" s="93" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D224" s="93" t="s">
         <v>19</v>
@@ -7463,7 +7460,7 @@
     </row>
     <row r="225">
       <c r="C225" s="93" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D225" s="93" t="s">
         <v>19</v>
@@ -7511,7 +7508,7 @@
     </row>
     <row r="227">
       <c r="C227" s="93" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D227" s="93" t="s">
         <v>19</v>
@@ -7535,7 +7532,7 @@
     </row>
     <row r="228">
       <c r="C228" s="93" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D228" s="93" t="s">
         <v>19</v>
@@ -7559,16 +7556,16 @@
     </row>
     <row r="229">
       <c r="C229" s="93" t="s">
+        <v>240</v>
+      </c>
+      <c r="D229" s="93" t="s">
+        <v>19</v>
+      </c>
+      <c r="E229" s="93" t="s">
+        <v>22</v>
+      </c>
+      <c r="F229" s="93" t="s">
         <v>241</v>
-      </c>
-      <c r="D229" s="93" t="s">
-        <v>19</v>
-      </c>
-      <c r="E229" s="93" t="s">
-        <v>22</v>
-      </c>
-      <c r="F229" s="93" t="s">
-        <v>242</v>
       </c>
       <c r="G229" s="93" t="s">
         <v>19</v>
@@ -7670,7 +7667,7 @@
     </row>
     <row r="234">
       <c r="A234" s="100" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B234" s="100" t="s">
         <v>19</v>
@@ -7724,7 +7721,7 @@
     </row>
     <row r="236">
       <c r="C236" s="99" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D236" s="99" t="s">
         <v>19</v>
@@ -7796,7 +7793,7 @@
     </row>
     <row r="239">
       <c r="C239" s="99" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D239" s="99" t="s">
         <v>19</v>
@@ -7820,7 +7817,7 @@
     </row>
     <row r="240">
       <c r="C240" s="99" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D240" s="99" t="s">
         <v>19</v>
@@ -7931,7 +7928,7 @@
     </row>
     <row r="245">
       <c r="A245" s="106" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B245" s="106" t="s">
         <v>19</v>
@@ -7961,7 +7958,7 @@
     </row>
     <row r="246">
       <c r="C246" s="105" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D246" s="105" t="s">
         <v>19</v>
@@ -8009,7 +8006,7 @@
     </row>
     <row r="248">
       <c r="C248" s="105" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D248" s="105" t="s">
         <v>19</v>
@@ -8174,19 +8171,19 @@
     </row>
     <row r="255">
       <c r="C255" s="111" t="s">
+        <v>249</v>
+      </c>
+      <c r="D255" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="E255" s="111" t="s">
+        <v>16</v>
+      </c>
+      <c r="F255" s="111" t="s">
+        <v>17</v>
+      </c>
+      <c r="G255" s="111" t="s">
         <v>250</v>
-      </c>
-      <c r="D255" s="111" t="s">
-        <v>19</v>
-      </c>
-      <c r="E255" s="111" t="s">
-        <v>16</v>
-      </c>
-      <c r="F255" s="111" t="s">
-        <v>17</v>
-      </c>
-      <c r="G255" s="111" t="s">
-        <v>251</v>
       </c>
       <c r="H255" s="111" t="s">
         <v>19</v>
@@ -8234,7 +8231,7 @@
         <v>17</v>
       </c>
       <c r="G257" s="111" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H257" s="111" t="s">
         <v>19</v>
@@ -8246,7 +8243,7 @@
     </row>
     <row r="258">
       <c r="C258" s="111" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D258" s="111" t="s">
         <v>19</v>
@@ -8270,7 +8267,7 @@
     </row>
     <row r="259">
       <c r="C259" s="111" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D259" s="111" t="s">
         <v>19</v>
@@ -8294,7 +8291,7 @@
     </row>
     <row r="260">
       <c r="C260" s="111" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D260" s="111" t="s">
         <v>19</v>
@@ -8405,7 +8402,7 @@
     </row>
     <row r="265">
       <c r="A265" s="118" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B265" s="118" t="s">
         <v>19</v>
@@ -8414,7 +8411,7 @@
         <v>14</v>
       </c>
       <c r="D265" s="117" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E265" s="117" t="s">
         <v>16</v>
@@ -8438,7 +8435,7 @@
         <v>20</v>
       </c>
       <c r="D266" s="117" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="E266" s="117" t="s">
         <v>16</v>
@@ -8459,10 +8456,10 @@
     </row>
     <row r="267">
       <c r="C267" s="117" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D267" s="117" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="E267" s="117" t="s">
         <v>22</v>
@@ -8483,19 +8480,19 @@
     </row>
     <row r="268">
       <c r="C268" s="117" t="s">
+        <v>256</v>
+      </c>
+      <c r="D268" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="E268" s="117" t="s">
+        <v>16</v>
+      </c>
+      <c r="F268" s="117" t="s">
+        <v>17</v>
+      </c>
+      <c r="G268" s="117" t="s">
         <v>257</v>
-      </c>
-      <c r="D268" s="117" t="s">
-        <v>190</v>
-      </c>
-      <c r="E268" s="117" t="s">
-        <v>16</v>
-      </c>
-      <c r="F268" s="117" t="s">
-        <v>17</v>
-      </c>
-      <c r="G268" s="117" t="s">
-        <v>258</v>
       </c>
       <c r="H268" s="117" t="s">
         <v>19</v>
@@ -8507,10 +8504,10 @@
     </row>
     <row r="269">
       <c r="C269" s="117" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D269" s="117" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="E269" s="117" t="s">
         <v>22</v>
@@ -8531,19 +8528,19 @@
     </row>
     <row r="270">
       <c r="C270" s="117" t="s">
+        <v>259</v>
+      </c>
+      <c r="D270" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="E270" s="117" t="s">
+        <v>16</v>
+      </c>
+      <c r="F270" s="117" t="s">
+        <v>17</v>
+      </c>
+      <c r="G270" s="117" t="s">
         <v>260</v>
-      </c>
-      <c r="D270" s="117" t="s">
-        <v>190</v>
-      </c>
-      <c r="E270" s="117" t="s">
-        <v>16</v>
-      </c>
-      <c r="F270" s="117" t="s">
-        <v>17</v>
-      </c>
-      <c r="G270" s="117" t="s">
-        <v>261</v>
       </c>
       <c r="H270" s="117" t="s">
         <v>19</v>
@@ -8555,11 +8552,11 @@
     </row>
     <row r="271">
       <c r="C271" s="117" t="s">
+        <v>261</v>
+      </c>
+      <c r="D271" s="117" t="s">
         <v>262</v>
       </c>
-      <c r="D271" s="117" t="s">
-        <v>263</v>
-      </c>
       <c r="E271" s="117" t="s">
         <v>22</v>
       </c>
@@ -8567,7 +8564,7 @@
         <v>17</v>
       </c>
       <c r="G271" s="117" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H271" s="117" t="s">
         <v>19</v>
@@ -8579,10 +8576,10 @@
     </row>
     <row r="272">
       <c r="C272" s="117" t="s">
+        <v>263</v>
+      </c>
+      <c r="D272" s="117" t="s">
         <v>264</v>
-      </c>
-      <c r="D272" s="117" t="s">
-        <v>265</v>
       </c>
       <c r="E272" s="117" t="s">
         <v>22</v>
@@ -8606,7 +8603,7 @@
         <v>82</v>
       </c>
       <c r="D273" s="117" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="E273" s="117" t="s">
         <v>22</v>
@@ -8630,7 +8627,7 @@
         <v>189</v>
       </c>
       <c r="D274" s="117" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="E274" s="117" t="s">
         <v>22</v>
@@ -8654,7 +8651,7 @@
         <v>36</v>
       </c>
       <c r="D275" s="117" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="E275" s="117" t="s">
         <v>16</v>
@@ -8680,7 +8677,7 @@
         <v>39</v>
       </c>
       <c r="D276" s="118" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="E276" s="118" t="s">
         <v>16</v>
@@ -8738,7 +8735,7 @@
     </row>
     <row r="279">
       <c r="A279" s="124" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B279" s="124" t="s">
         <v>19</v>
@@ -8816,7 +8813,7 @@
     </row>
     <row r="282">
       <c r="C282" s="123" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D282" s="123" t="s">
         <v>19</v>
@@ -8840,7 +8837,7 @@
     </row>
     <row r="283">
       <c r="C283" s="123" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D283" s="123" t="s">
         <v>19</v>
@@ -8864,7 +8861,7 @@
     </row>
     <row r="284">
       <c r="C284" s="123" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D284" s="123" t="s">
         <v>19</v>
@@ -8888,7 +8885,7 @@
     </row>
     <row r="285">
       <c r="C285" s="123" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D285" s="123" t="s">
         <v>19</v>
@@ -8912,7 +8909,7 @@
     </row>
     <row r="286">
       <c r="C286" s="123" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D286" s="123" t="s">
         <v>19</v>
@@ -8936,7 +8933,7 @@
     </row>
     <row r="287">
       <c r="C287" s="123" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D287" s="123" t="s">
         <v>19</v>
@@ -8960,7 +8957,7 @@
     </row>
     <row r="288">
       <c r="C288" s="123" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D288" s="123" t="s">
         <v>19</v>
@@ -8984,7 +8981,7 @@
     </row>
     <row r="289">
       <c r="C289" s="123" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D289" s="123" t="s">
         <v>19</v>
@@ -9008,7 +9005,7 @@
     </row>
     <row r="290">
       <c r="C290" s="123" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D290" s="123" t="s">
         <v>19</v>
@@ -9032,7 +9029,7 @@
     </row>
     <row r="291">
       <c r="C291" s="123" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D291" s="123" t="s">
         <v>19</v>
@@ -9056,7 +9053,7 @@
     </row>
     <row r="292">
       <c r="C292" s="123" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D292" s="123" t="s">
         <v>19</v>
@@ -9080,7 +9077,7 @@
     </row>
     <row r="293">
       <c r="C293" s="123" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D293" s="123" t="s">
         <v>19</v>
@@ -9104,7 +9101,7 @@
     </row>
     <row r="294">
       <c r="C294" s="123" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D294" s="123" t="s">
         <v>19</v>
@@ -9215,7 +9212,7 @@
     </row>
     <row r="299">
       <c r="A299" s="130" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B299" s="130" t="s">
         <v>19</v>
@@ -9293,7 +9290,7 @@
     </row>
     <row r="302">
       <c r="C302" s="129" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D302" s="129" t="s">
         <v>19</v>
@@ -9317,7 +9314,7 @@
     </row>
     <row r="303">
       <c r="C303" s="129" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D303" s="129" t="s">
         <v>19</v>
@@ -9341,7 +9338,7 @@
     </row>
     <row r="304">
       <c r="C304" s="129" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D304" s="129" t="s">
         <v>19</v>
@@ -9365,7 +9362,7 @@
     </row>
     <row r="305">
       <c r="C305" s="129" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D305" s="129" t="s">
         <v>19</v>
@@ -9389,7 +9386,7 @@
     </row>
     <row r="306">
       <c r="C306" s="129" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D306" s="129" t="s">
         <v>19</v>
@@ -9413,7 +9410,7 @@
     </row>
     <row r="307">
       <c r="C307" s="129" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D307" s="129" t="s">
         <v>19</v>
@@ -9437,7 +9434,7 @@
     </row>
     <row r="308">
       <c r="C308" s="129" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D308" s="129" t="s">
         <v>19</v>
@@ -9461,7 +9458,7 @@
     </row>
     <row r="309">
       <c r="C309" s="129" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D309" s="129" t="s">
         <v>19</v>
@@ -9485,7 +9482,7 @@
     </row>
     <row r="310">
       <c r="C310" s="129" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D310" s="129" t="s">
         <v>19</v>
@@ -9509,7 +9506,7 @@
     </row>
     <row r="311">
       <c r="C311" s="129" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D311" s="129" t="s">
         <v>19</v>
@@ -9533,7 +9530,7 @@
     </row>
     <row r="312">
       <c r="C312" s="129" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D312" s="129" t="s">
         <v>19</v>
@@ -9557,7 +9554,7 @@
     </row>
     <row r="313">
       <c r="C313" s="129" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D313" s="129" t="s">
         <v>19</v>
@@ -9583,7 +9580,7 @@
       <c r="A314" s="130"/>
       <c r="B314" s="130"/>
       <c r="C314" s="130" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D314" s="130" t="s">
         <v>19</v>
@@ -9644,7 +9641,7 @@
     </row>
     <row r="317">
       <c r="A317" s="136" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B317" s="136" t="s">
         <v>19</v>
@@ -9698,7 +9695,7 @@
     </row>
     <row r="319">
       <c r="C319" s="135" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D319" s="135" t="s">
         <v>19</v>
@@ -9722,7 +9719,7 @@
     </row>
     <row r="320">
       <c r="C320" s="135" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D320" s="135" t="s">
         <v>19</v>
@@ -9746,7 +9743,7 @@
     </row>
     <row r="321">
       <c r="C321" s="135" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D321" s="135" t="s">
         <v>19</v>
@@ -9770,19 +9767,19 @@
     </row>
     <row r="322">
       <c r="C322" s="135" t="s">
+        <v>295</v>
+      </c>
+      <c r="D322" s="135" t="s">
+        <v>19</v>
+      </c>
+      <c r="E322" s="135" t="s">
+        <v>16</v>
+      </c>
+      <c r="F322" s="135" t="s">
+        <v>17</v>
+      </c>
+      <c r="G322" s="135" t="s">
         <v>296</v>
-      </c>
-      <c r="D322" s="135" t="s">
-        <v>19</v>
-      </c>
-      <c r="E322" s="135" t="s">
-        <v>16</v>
-      </c>
-      <c r="F322" s="135" t="s">
-        <v>17</v>
-      </c>
-      <c r="G322" s="135" t="s">
-        <v>297</v>
       </c>
       <c r="H322" s="135" t="s">
         <v>19</v>
@@ -9794,7 +9791,7 @@
     </row>
     <row r="323">
       <c r="C323" s="135" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D323" s="135" t="s">
         <v>19</v>
@@ -9905,7 +9902,7 @@
     </row>
     <row r="328">
       <c r="A328" s="142" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B328" s="142" t="s">
         <v>19</v>
@@ -9935,7 +9932,7 @@
     </row>
     <row r="329">
       <c r="C329" s="141" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D329" s="141" t="s">
         <v>19</v>
@@ -9959,7 +9956,7 @@
     </row>
     <row r="330">
       <c r="C330" s="141" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D330" s="141" t="s">
         <v>19</v>
@@ -10070,7 +10067,7 @@
     </row>
     <row r="335">
       <c r="A335" s="148" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B335" s="148" t="s">
         <v>19</v>
@@ -10172,7 +10169,7 @@
     </row>
     <row r="339">
       <c r="C339" s="147" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D339" s="147" t="s">
         <v>19</v>
@@ -10184,7 +10181,7 @@
         <v>17</v>
       </c>
       <c r="G339" s="147" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H339" s="147" t="s">
         <v>19</v>
@@ -10196,7 +10193,7 @@
     </row>
     <row r="340">
       <c r="C340" s="147" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D340" s="147" t="s">
         <v>19</v>
@@ -10283,7 +10280,7 @@
     </row>
     <row r="344">
       <c r="A344" s="154" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B344" s="154" t="s">
         <v>19</v>
@@ -10361,7 +10358,7 @@
     </row>
     <row r="347">
       <c r="C347" s="153" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D347" s="153" t="s">
         <v>19</v>
@@ -10385,7 +10382,7 @@
     </row>
     <row r="348">
       <c r="C348" s="153" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D348" s="153" t="s">
         <v>19</v>
@@ -10409,7 +10406,7 @@
     </row>
     <row r="349">
       <c r="C349" s="153" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D349" s="153" t="s">
         <v>19</v>
@@ -10433,7 +10430,7 @@
     </row>
     <row r="350">
       <c r="C350" s="153" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D350" s="153" t="s">
         <v>19</v>
@@ -10457,7 +10454,7 @@
     </row>
     <row r="351">
       <c r="C351" s="153" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D351" s="153" t="s">
         <v>19</v>
@@ -10568,7 +10565,7 @@
     </row>
     <row r="356">
       <c r="A356" s="160" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B356" s="160" t="s">
         <v>19</v>
@@ -10577,7 +10574,7 @@
         <v>14</v>
       </c>
       <c r="D356" s="159" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E356" s="159" t="s">
         <v>16</v>
@@ -10601,7 +10598,7 @@
         <v>20</v>
       </c>
       <c r="D357" s="159" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E357" s="159" t="s">
         <v>16</v>
@@ -10625,7 +10622,7 @@
         <v>86</v>
       </c>
       <c r="D358" s="159" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E358" s="159" t="s">
         <v>16</v>
@@ -10649,7 +10646,7 @@
         <v>87</v>
       </c>
       <c r="D359" s="159" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E359" s="159" t="s">
         <v>22</v>
@@ -10670,10 +10667,10 @@
     </row>
     <row r="360">
       <c r="C360" s="159" t="s">
+        <v>310</v>
+      </c>
+      <c r="D360" s="159" t="s">
         <v>311</v>
-      </c>
-      <c r="D360" s="159" t="s">
-        <v>312</v>
       </c>
       <c r="E360" s="159" t="s">
         <v>22</v>
@@ -10697,7 +10694,7 @@
         <v>89</v>
       </c>
       <c r="D361" s="159" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E361" s="159" t="s">
         <v>22</v>
@@ -10721,7 +10718,7 @@
         <v>67</v>
       </c>
       <c r="D362" s="159" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E362" s="159" t="s">
         <v>22</v>
@@ -10745,7 +10742,7 @@
         <v>91</v>
       </c>
       <c r="D363" s="159" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E363" s="159" t="s">
         <v>22</v>
@@ -10769,7 +10766,7 @@
         <v>92</v>
       </c>
       <c r="D364" s="159" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E364" s="159" t="s">
         <v>22</v>
@@ -10790,10 +10787,10 @@
     </row>
     <row r="365">
       <c r="C365" s="159" t="s">
+        <v>315</v>
+      </c>
+      <c r="D365" s="159" t="s">
         <v>316</v>
-      </c>
-      <c r="D365" s="159" t="s">
-        <v>317</v>
       </c>
       <c r="E365" s="159" t="s">
         <v>22</v>
@@ -10817,7 +10814,7 @@
         <v>93</v>
       </c>
       <c r="D366" s="159" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E366" s="159" t="s">
         <v>22</v>
@@ -10838,10 +10835,10 @@
     </row>
     <row r="367">
       <c r="C367" s="159" t="s">
+        <v>318</v>
+      </c>
+      <c r="D367" s="159" t="s">
         <v>319</v>
-      </c>
-      <c r="D367" s="159" t="s">
-        <v>320</v>
       </c>
       <c r="E367" s="159" t="s">
         <v>22</v>
@@ -10865,7 +10862,7 @@
         <v>94</v>
       </c>
       <c r="D368" s="159" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E368" s="159" t="s">
         <v>22</v>
@@ -10889,7 +10886,7 @@
         <v>95</v>
       </c>
       <c r="D369" s="159" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E369" s="159" t="s">
         <v>16</v>
@@ -10913,7 +10910,7 @@
         <v>97</v>
       </c>
       <c r="D370" s="159" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E370" s="159" t="s">
         <v>16</v>
@@ -10937,7 +10934,7 @@
         <v>99</v>
       </c>
       <c r="D371" s="159" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E371" s="159" t="s">
         <v>16</v>
@@ -10961,7 +10958,7 @@
         <v>100</v>
       </c>
       <c r="D372" s="159" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E372" s="159" t="s">
         <v>16</v>
@@ -10985,7 +10982,7 @@
         <v>101</v>
       </c>
       <c r="D373" s="159" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E373" s="159" t="s">
         <v>22</v>
@@ -11009,7 +11006,7 @@
         <v>102</v>
       </c>
       <c r="D374" s="159" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E374" s="159" t="s">
         <v>22</v>
@@ -11033,7 +11030,7 @@
         <v>103</v>
       </c>
       <c r="D375" s="159" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E375" s="159" t="s">
         <v>22</v>
@@ -11057,7 +11054,7 @@
         <v>104</v>
       </c>
       <c r="D376" s="159" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E376" s="159" t="s">
         <v>22</v>
@@ -11081,7 +11078,7 @@
         <v>105</v>
       </c>
       <c r="D377" s="159" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E377" s="159" t="s">
         <v>22</v>
@@ -11105,7 +11102,7 @@
         <v>106</v>
       </c>
       <c r="D378" s="159" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E378" s="159" t="s">
         <v>22</v>
@@ -11129,7 +11126,7 @@
         <v>107</v>
       </c>
       <c r="D379" s="159" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E379" s="159" t="s">
         <v>16</v>
@@ -11153,7 +11150,7 @@
         <v>108</v>
       </c>
       <c r="D380" s="159" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E380" s="159" t="s">
         <v>16</v>
@@ -11177,7 +11174,7 @@
         <v>109</v>
       </c>
       <c r="D381" s="159" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E381" s="159" t="s">
         <v>16</v>
@@ -11201,7 +11198,7 @@
         <v>111</v>
       </c>
       <c r="D382" s="159" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E382" s="159" t="s">
         <v>16</v>
@@ -11225,7 +11222,7 @@
         <v>112</v>
       </c>
       <c r="D383" s="159" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E383" s="159" t="s">
         <v>16</v>
@@ -11249,7 +11246,7 @@
         <v>113</v>
       </c>
       <c r="D384" s="159" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E384" s="159" t="s">
         <v>16</v>
@@ -11273,7 +11270,7 @@
         <v>114</v>
       </c>
       <c r="D385" s="159" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E385" s="159" t="s">
         <v>22</v>
@@ -11297,7 +11294,7 @@
         <v>115</v>
       </c>
       <c r="D386" s="159" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E386" s="159" t="s">
         <v>16</v>
@@ -11321,7 +11318,7 @@
         <v>116</v>
       </c>
       <c r="D387" s="159" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E387" s="159" t="s">
         <v>16</v>
@@ -11345,7 +11342,7 @@
         <v>117</v>
       </c>
       <c r="D388" s="159" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E388" s="159" t="s">
         <v>16</v>
@@ -11369,7 +11366,7 @@
         <v>118</v>
       </c>
       <c r="D389" s="159" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E389" s="159" t="s">
         <v>16</v>
@@ -11393,7 +11390,7 @@
         <v>119</v>
       </c>
       <c r="D390" s="159" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E390" s="159" t="s">
         <v>16</v>
@@ -11417,7 +11414,7 @@
         <v>120</v>
       </c>
       <c r="D391" s="159" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E391" s="159" t="s">
         <v>22</v>
@@ -11441,7 +11438,7 @@
         <v>121</v>
       </c>
       <c r="D392" s="159" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E392" s="159" t="s">
         <v>22</v>
@@ -11465,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="D393" s="159" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E393" s="159" t="s">
         <v>22</v>
@@ -11489,7 +11486,7 @@
         <v>36</v>
       </c>
       <c r="D394" s="159" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E394" s="159" t="s">
         <v>16</v>
@@ -11513,7 +11510,7 @@
         <v>39</v>
       </c>
       <c r="D395" s="159" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E395" s="159" t="s">
         <v>16</v>
@@ -11537,7 +11534,7 @@
         <v>128</v>
       </c>
       <c r="D396" s="159" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E396" s="159" t="s">
         <v>22</v>
@@ -11561,7 +11558,7 @@
         <v>129</v>
       </c>
       <c r="D397" s="159" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E397" s="159" t="s">
         <v>22</v>
@@ -11585,7 +11582,7 @@
         <v>130</v>
       </c>
       <c r="D398" s="159" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E398" s="159" t="s">
         <v>22</v>
@@ -11609,7 +11606,7 @@
         <v>131</v>
       </c>
       <c r="D399" s="159" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E399" s="159" t="s">
         <v>22</v>
@@ -11633,7 +11630,7 @@
         <v>132</v>
       </c>
       <c r="D400" s="159" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E400" s="159" t="s">
         <v>22</v>
@@ -11654,10 +11651,10 @@
     </row>
     <row r="401">
       <c r="C401" s="159" t="s">
+        <v>352</v>
+      </c>
+      <c r="D401" s="159" t="s">
         <v>353</v>
-      </c>
-      <c r="D401" s="159" t="s">
-        <v>354</v>
       </c>
       <c r="E401" s="159" t="s">
         <v>22</v>
@@ -11678,10 +11675,10 @@
     </row>
     <row r="402">
       <c r="C402" s="159" t="s">
+        <v>354</v>
+      </c>
+      <c r="D402" s="159" t="s">
         <v>355</v>
-      </c>
-      <c r="D402" s="159" t="s">
-        <v>356</v>
       </c>
       <c r="E402" s="159" t="s">
         <v>22</v>
@@ -11702,10 +11699,10 @@
     </row>
     <row r="403">
       <c r="C403" s="159" t="s">
+        <v>356</v>
+      </c>
+      <c r="D403" s="159" t="s">
         <v>357</v>
-      </c>
-      <c r="D403" s="159" t="s">
-        <v>358</v>
       </c>
       <c r="E403" s="159" t="s">
         <v>22</v>
@@ -11728,7 +11725,7 @@
       <c r="A404" s="160"/>
       <c r="B404" s="160"/>
       <c r="C404" s="160" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D404" s="160" t="s">
         <v>19</v>
@@ -11789,25 +11786,25 @@
     </row>
     <row r="407">
       <c r="A407" s="166" t="s">
+        <v>359</v>
+      </c>
+      <c r="B407" s="166" t="s">
+        <v>19</v>
+      </c>
+      <c r="C407" s="165" t="s">
         <v>360</v>
       </c>
-      <c r="B407" s="166" t="s">
-        <v>19</v>
-      </c>
-      <c r="C407" s="165" t="s">
+      <c r="D407" s="165" t="s">
+        <v>19</v>
+      </c>
+      <c r="E407" s="165" t="s">
+        <v>16</v>
+      </c>
+      <c r="F407" s="165" t="s">
+        <v>17</v>
+      </c>
+      <c r="G407" s="165" t="s">
         <v>361</v>
-      </c>
-      <c r="D407" s="165" t="s">
-        <v>19</v>
-      </c>
-      <c r="E407" s="165" t="s">
-        <v>16</v>
-      </c>
-      <c r="F407" s="165" t="s">
-        <v>17</v>
-      </c>
-      <c r="G407" s="165" t="s">
-        <v>362</v>
       </c>
       <c r="H407" s="165" t="s">
         <v>8</v>
@@ -11821,7 +11818,7 @@
       <c r="A408" s="166"/>
       <c r="B408" s="166"/>
       <c r="C408" s="166" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D408" s="166" t="s">
         <v>19</v>
@@ -11833,7 +11830,7 @@
         <v>17</v>
       </c>
       <c r="G408" s="166" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H408" s="166" t="s">
         <v>19</v>
@@ -11882,7 +11879,7 @@
     </row>
     <row r="411">
       <c r="A411" s="172" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B411" s="172" t="s">
         <v>19</v>
@@ -11912,19 +11909,19 @@
     </row>
     <row r="412">
       <c r="C412" s="171" t="s">
+        <v>360</v>
+      </c>
+      <c r="D412" s="171" t="s">
+        <v>19</v>
+      </c>
+      <c r="E412" s="171" t="s">
+        <v>16</v>
+      </c>
+      <c r="F412" s="171" t="s">
+        <v>17</v>
+      </c>
+      <c r="G412" s="171" t="s">
         <v>361</v>
-      </c>
-      <c r="D412" s="171" t="s">
-        <v>19</v>
-      </c>
-      <c r="E412" s="171" t="s">
-        <v>16</v>
-      </c>
-      <c r="F412" s="171" t="s">
-        <v>17</v>
-      </c>
-      <c r="G412" s="171" t="s">
-        <v>362</v>
       </c>
       <c r="H412" s="171" t="s">
         <v>19</v>
@@ -11936,7 +11933,7 @@
     </row>
     <row r="413">
       <c r="C413" s="171" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D413" s="171" t="s">
         <v>19</v>
@@ -11948,7 +11945,7 @@
         <v>17</v>
       </c>
       <c r="G413" s="171" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H413" s="171" t="s">
         <v>19</v>
@@ -11960,7 +11957,7 @@
     </row>
     <row r="414">
       <c r="C414" s="171" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D414" s="171" t="s">
         <v>19</v>
@@ -11972,7 +11969,7 @@
         <v>17</v>
       </c>
       <c r="G414" s="171" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H414" s="171" t="s">
         <v>19</v>
@@ -11984,19 +11981,19 @@
     </row>
     <row r="415">
       <c r="C415" s="171" t="s">
+        <v>366</v>
+      </c>
+      <c r="D415" s="171" t="s">
+        <v>19</v>
+      </c>
+      <c r="E415" s="171" t="s">
+        <v>16</v>
+      </c>
+      <c r="F415" s="171" t="s">
+        <v>17</v>
+      </c>
+      <c r="G415" s="171" t="s">
         <v>367</v>
-      </c>
-      <c r="D415" s="171" t="s">
-        <v>19</v>
-      </c>
-      <c r="E415" s="171" t="s">
-        <v>16</v>
-      </c>
-      <c r="F415" s="171" t="s">
-        <v>17</v>
-      </c>
-      <c r="G415" s="171" t="s">
-        <v>368</v>
       </c>
       <c r="H415" s="171" t="s">
         <v>19</v>
@@ -12010,7 +12007,7 @@
       <c r="A416" s="172"/>
       <c r="B416" s="172"/>
       <c r="C416" s="172" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D416" s="172" t="s">
         <v>19</v>
@@ -12022,7 +12019,7 @@
         <v>17</v>
       </c>
       <c r="G416" s="172" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H416" s="172" t="s">
         <v>19</v>
@@ -12071,7 +12068,7 @@
     </row>
     <row r="419">
       <c r="A419" s="178" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B419" s="178" t="s">
         <v>19</v>
@@ -12125,7 +12122,7 @@
     </row>
     <row r="421">
       <c r="C421" s="177" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D421" s="177" t="s">
         <v>19</v>
@@ -12149,7 +12146,7 @@
     </row>
     <row r="422">
       <c r="C422" s="177" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D422" s="177" t="s">
         <v>19</v>
@@ -12161,7 +12158,7 @@
         <v>17</v>
       </c>
       <c r="G422" s="177" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H422" s="177" t="s">
         <v>19</v>
@@ -12173,7 +12170,7 @@
     </row>
     <row r="423">
       <c r="C423" s="177" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D423" s="177" t="s">
         <v>19</v>
@@ -12260,7 +12257,7 @@
     </row>
     <row r="427">
       <c r="A427" s="184" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B427" s="184" t="s">
         <v>19</v>
@@ -12290,10 +12287,10 @@
     </row>
     <row r="428">
       <c r="C428" s="183" t="s">
+        <v>371</v>
+      </c>
+      <c r="D428" s="183" t="s">
         <v>372</v>
-      </c>
-      <c r="D428" s="183" t="s">
-        <v>373</v>
       </c>
       <c r="E428" s="183" t="s">
         <v>16</v>
@@ -12317,7 +12314,7 @@
         <v>166</v>
       </c>
       <c r="D429" s="183" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E429" s="183" t="s">
         <v>22</v>
@@ -12338,10 +12335,10 @@
     </row>
     <row r="430">
       <c r="C430" s="183" t="s">
+        <v>374</v>
+      </c>
+      <c r="D430" s="183" t="s">
         <v>375</v>
-      </c>
-      <c r="D430" s="183" t="s">
-        <v>376</v>
       </c>
       <c r="E430" s="183" t="s">
         <v>22</v>
@@ -12362,11 +12359,11 @@
     </row>
     <row r="431">
       <c r="C431" s="183" t="s">
+        <v>376</v>
+      </c>
+      <c r="D431" s="183" t="s">
         <v>377</v>
       </c>
-      <c r="D431" s="183" t="s">
-        <v>378</v>
-      </c>
       <c r="E431" s="183" t="s">
         <v>22</v>
       </c>
@@ -12374,7 +12371,7 @@
         <v>17</v>
       </c>
       <c r="G431" s="183" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H431" s="183" t="s">
         <v>19</v>
@@ -12386,10 +12383,10 @@
     </row>
     <row r="432">
       <c r="C432" s="183" t="s">
+        <v>378</v>
+      </c>
+      <c r="D432" s="183" t="s">
         <v>379</v>
-      </c>
-      <c r="D432" s="183" t="s">
-        <v>380</v>
       </c>
       <c r="E432" s="183" t="s">
         <v>16</v>
@@ -12497,7 +12494,7 @@
     </row>
     <row r="437">
       <c r="A437" s="190" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B437" s="190" t="s">
         <v>19</v>
@@ -12527,16 +12524,16 @@
     </row>
     <row r="438">
       <c r="C438" s="189" t="s">
+        <v>381</v>
+      </c>
+      <c r="D438" s="189" t="s">
+        <v>19</v>
+      </c>
+      <c r="E438" s="189" t="s">
+        <v>22</v>
+      </c>
+      <c r="F438" s="189" t="s">
         <v>382</v>
-      </c>
-      <c r="D438" s="189" t="s">
-        <v>19</v>
-      </c>
-      <c r="E438" s="189" t="s">
-        <v>22</v>
-      </c>
-      <c r="F438" s="189" t="s">
-        <v>383</v>
       </c>
       <c r="G438" s="189" t="s">
         <v>19</v>
@@ -12551,7 +12548,7 @@
     </row>
     <row r="439">
       <c r="C439" s="189" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D439" s="189" t="s">
         <v>19</v>
@@ -12575,7 +12572,7 @@
     </row>
     <row r="440">
       <c r="C440" s="189" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D440" s="189" t="s">
         <v>19</v>
@@ -12686,7 +12683,7 @@
     </row>
     <row r="445">
       <c r="A445" s="196" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B445" s="196" t="s">
         <v>19</v>
@@ -12716,7 +12713,7 @@
     </row>
     <row r="446">
       <c r="C446" s="195" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D446" s="195" t="s">
         <v>19</v>
@@ -12740,7 +12737,7 @@
     </row>
     <row r="447">
       <c r="C447" s="195" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D447" s="195" t="s">
         <v>19</v>
@@ -12764,16 +12761,16 @@
     </row>
     <row r="448">
       <c r="C448" s="195" t="s">
+        <v>385</v>
+      </c>
+      <c r="D448" s="195" t="s">
+        <v>19</v>
+      </c>
+      <c r="E448" s="195" t="s">
+        <v>16</v>
+      </c>
+      <c r="F448" s="195" t="s">
         <v>386</v>
-      </c>
-      <c r="D448" s="195" t="s">
-        <v>19</v>
-      </c>
-      <c r="E448" s="195" t="s">
-        <v>16</v>
-      </c>
-      <c r="F448" s="195" t="s">
-        <v>387</v>
       </c>
       <c r="G448" s="195" t="s">
         <v>19</v>
@@ -12875,7 +12872,7 @@
     </row>
     <row r="453">
       <c r="A453" s="202" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B453" s="202" t="s">
         <v>19</v>
@@ -12905,7 +12902,7 @@
     </row>
     <row r="454">
       <c r="C454" s="201" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D454" s="201" t="s">
         <v>19</v>
@@ -12914,7 +12911,7 @@
         <v>22</v>
       </c>
       <c r="F454" s="201" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G454" s="201" t="s">
         <v>19</v>
@@ -12929,7 +12926,7 @@
     </row>
     <row r="455">
       <c r="C455" s="201" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D455" s="201" t="s">
         <v>19</v>
@@ -12941,7 +12938,7 @@
         <v>17</v>
       </c>
       <c r="G455" s="201" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H455" s="201" t="s">
         <v>19</v>
@@ -13040,7 +13037,7 @@
     </row>
     <row r="460">
       <c r="A460" s="208" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B460" s="208" t="s">
         <v>19</v>
@@ -13070,7 +13067,7 @@
     </row>
     <row r="461">
       <c r="C461" s="207" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D461" s="207" t="s">
         <v>19</v>
@@ -13082,7 +13079,7 @@
         <v>17</v>
       </c>
       <c r="G461" s="207" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H461" s="207" t="s">
         <v>19</v>
@@ -13094,7 +13091,7 @@
     </row>
     <row r="462">
       <c r="C462" s="207" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D462" s="207" t="s">
         <v>19</v>
@@ -13307,7 +13304,7 @@
     </row>
     <row r="471">
       <c r="C471" s="213" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D471" s="213" t="s">
         <v>19</v>
@@ -13331,7 +13328,7 @@
     </row>
     <row r="472">
       <c r="C472" s="213" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D472" s="213" t="s">
         <v>19</v>
@@ -13355,7 +13352,7 @@
     </row>
     <row r="473">
       <c r="C473" s="213" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D473" s="213" t="s">
         <v>19</v>
@@ -13379,7 +13376,7 @@
     </row>
     <row r="474">
       <c r="C474" s="213" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D474" s="213" t="s">
         <v>19</v>
@@ -13403,7 +13400,7 @@
     </row>
     <row r="475">
       <c r="C475" s="213" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D475" s="213" t="s">
         <v>19</v>
@@ -13427,7 +13424,7 @@
     </row>
     <row r="476">
       <c r="C476" s="213" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D476" s="213" t="s">
         <v>19</v>
@@ -13451,7 +13448,7 @@
     </row>
     <row r="477">
       <c r="C477" s="213" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D477" s="213" t="s">
         <v>19</v>
@@ -13475,7 +13472,7 @@
     </row>
     <row r="478">
       <c r="C478" s="213" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D478" s="213" t="s">
         <v>19</v>
@@ -13499,7 +13496,7 @@
     </row>
     <row r="479">
       <c r="C479" s="213" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D479" s="213" t="s">
         <v>19</v>
@@ -13523,7 +13520,7 @@
     </row>
     <row r="480">
       <c r="C480" s="213" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D480" s="213" t="s">
         <v>19</v>
@@ -13658,7 +13655,7 @@
     </row>
     <row r="486">
       <c r="A486" s="220" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B486" s="220" t="s">
         <v>19</v>
@@ -13736,7 +13733,7 @@
     </row>
     <row r="489">
       <c r="C489" s="219" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D489" s="219" t="s">
         <v>19</v>
@@ -13760,7 +13757,7 @@
     </row>
     <row r="490">
       <c r="C490" s="219" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D490" s="219" t="s">
         <v>19</v>
@@ -13784,7 +13781,7 @@
     </row>
     <row r="491">
       <c r="C491" s="219" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D491" s="219" t="s">
         <v>19</v>
@@ -13895,7 +13892,7 @@
     </row>
     <row r="496">
       <c r="A496" s="226" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B496" s="226" t="s">
         <v>19</v>
@@ -13904,7 +13901,7 @@
         <v>14</v>
       </c>
       <c r="D496" s="225" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E496" s="225" t="s">
         <v>16</v>
@@ -13949,10 +13946,10 @@
     </row>
     <row r="498">
       <c r="C498" s="225" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D498" s="225" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E498" s="225" t="s">
         <v>22</v>
@@ -13978,7 +13975,7 @@
         <v>82</v>
       </c>
       <c r="D499" s="226" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E499" s="226" t="s">
         <v>16</v>
@@ -14036,7 +14033,7 @@
     </row>
     <row r="502">
       <c r="A502" s="232" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B502" s="232" t="s">
         <v>19</v>
@@ -14045,7 +14042,7 @@
         <v>14</v>
       </c>
       <c r="D502" s="231" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E502" s="231" t="s">
         <v>16</v>
@@ -14093,7 +14090,7 @@
         <v>29</v>
       </c>
       <c r="D504" s="231" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E504" s="231" t="s">
         <v>22</v>
@@ -14114,10 +14111,10 @@
     </row>
     <row r="505">
       <c r="C505" s="231" t="s">
+        <v>411</v>
+      </c>
+      <c r="D505" s="231" t="s">
         <v>412</v>
-      </c>
-      <c r="D505" s="231" t="s">
-        <v>413</v>
       </c>
       <c r="E505" s="231" t="s">
         <v>22</v>
@@ -14138,16 +14135,16 @@
     </row>
     <row r="506">
       <c r="C506" s="231" t="s">
+        <v>413</v>
+      </c>
+      <c r="D506" s="231" t="s">
         <v>414</v>
       </c>
-      <c r="D506" s="231" t="s">
-        <v>415</v>
-      </c>
       <c r="E506" s="231" t="s">
         <v>22</v>
       </c>
       <c r="F506" s="231" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G506" s="231" t="s">
         <v>19</v>
@@ -14162,16 +14159,16 @@
     </row>
     <row r="507">
       <c r="C507" s="231" t="s">
+        <v>415</v>
+      </c>
+      <c r="D507" s="231" t="s">
         <v>416</v>
       </c>
-      <c r="D507" s="231" t="s">
-        <v>417</v>
-      </c>
       <c r="E507" s="231" t="s">
         <v>22</v>
       </c>
       <c r="F507" s="231" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G507" s="231" t="s">
         <v>19</v>
@@ -14186,16 +14183,16 @@
     </row>
     <row r="508">
       <c r="C508" s="231" t="s">
+        <v>417</v>
+      </c>
+      <c r="D508" s="231" t="s">
         <v>418</v>
       </c>
-      <c r="D508" s="231" t="s">
-        <v>419</v>
-      </c>
       <c r="E508" s="231" t="s">
         <v>22</v>
       </c>
       <c r="F508" s="231" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G508" s="231" t="s">
         <v>19</v>
@@ -14210,10 +14207,10 @@
     </row>
     <row r="509">
       <c r="C509" s="231" t="s">
+        <v>419</v>
+      </c>
+      <c r="D509" s="231" t="s">
         <v>420</v>
-      </c>
-      <c r="D509" s="231" t="s">
-        <v>421</v>
       </c>
       <c r="E509" s="231" t="s">
         <v>22</v>
@@ -14234,10 +14231,10 @@
     </row>
     <row r="510">
       <c r="C510" s="231" t="s">
+        <v>421</v>
+      </c>
+      <c r="D510" s="231" t="s">
         <v>422</v>
-      </c>
-      <c r="D510" s="231" t="s">
-        <v>423</v>
       </c>
       <c r="E510" s="231" t="s">
         <v>22</v>
@@ -14261,7 +14258,7 @@
         <v>82</v>
       </c>
       <c r="D511" s="231" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E511" s="231" t="s">
         <v>22</v>
@@ -14285,7 +14282,7 @@
         <v>36</v>
       </c>
       <c r="D512" s="231" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E512" s="231" t="s">
         <v>22</v>
@@ -14311,7 +14308,7 @@
         <v>39</v>
       </c>
       <c r="D513" s="232" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E513" s="232" t="s">
         <v>22</v>
@@ -14369,7 +14366,7 @@
     </row>
     <row r="516">
       <c r="A516" s="238" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B516" s="238" t="s">
         <v>19</v>
@@ -14378,7 +14375,7 @@
         <v>14</v>
       </c>
       <c r="D516" s="237" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E516" s="237" t="s">
         <v>16</v>
@@ -14426,7 +14423,7 @@
         <v>67</v>
       </c>
       <c r="D518" s="237" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E518" s="237" t="s">
         <v>22</v>
@@ -14447,10 +14444,10 @@
     </row>
     <row r="519">
       <c r="C519" s="237" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D519" s="237" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E519" s="237" t="s">
         <v>22</v>
@@ -14474,7 +14471,7 @@
         <v>82</v>
       </c>
       <c r="D520" s="237" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E520" s="237" t="s">
         <v>22</v>
@@ -14498,7 +14495,7 @@
         <v>72</v>
       </c>
       <c r="D521" s="237" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E521" s="237" t="s">
         <v>22</v>
@@ -14522,7 +14519,7 @@
         <v>86</v>
       </c>
       <c r="D522" s="237" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E522" s="237" t="s">
         <v>22</v>
@@ -14546,7 +14543,7 @@
         <v>36</v>
       </c>
       <c r="D523" s="237" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E523" s="237" t="s">
         <v>22</v>
@@ -14572,7 +14569,7 @@
         <v>39</v>
       </c>
       <c r="D524" s="238" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E524" s="238" t="s">
         <v>22</v>
@@ -14639,7 +14636,7 @@
         <v>14</v>
       </c>
       <c r="D527" s="243" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E527" s="243" t="s">
         <v>16</v>
@@ -14684,16 +14681,16 @@
     </row>
     <row r="529">
       <c r="C529" s="243" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D529" s="243" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E529" s="243" t="s">
         <v>22</v>
       </c>
       <c r="F529" s="243" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G529" s="243" t="s">
         <v>19</v>
@@ -14711,7 +14708,7 @@
         <v>67</v>
       </c>
       <c r="D530" s="243" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E530" s="243" t="s">
         <v>22</v>
@@ -14732,10 +14729,10 @@
     </row>
     <row r="531">
       <c r="C531" s="243" t="s">
+        <v>437</v>
+      </c>
+      <c r="D531" s="243" t="s">
         <v>438</v>
-      </c>
-      <c r="D531" s="243" t="s">
-        <v>439</v>
       </c>
       <c r="E531" s="243" t="s">
         <v>22</v>
@@ -14756,10 +14753,10 @@
     </row>
     <row r="532">
       <c r="C532" s="243" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D532" s="243" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E532" s="243" t="s">
         <v>22</v>
@@ -14780,10 +14777,10 @@
     </row>
     <row r="533">
       <c r="C533" s="243" t="s">
+        <v>440</v>
+      </c>
+      <c r="D533" s="243" t="s">
         <v>441</v>
-      </c>
-      <c r="D533" s="243" t="s">
-        <v>442</v>
       </c>
       <c r="E533" s="243" t="s">
         <v>22</v>
@@ -14804,10 +14801,10 @@
     </row>
     <row r="534">
       <c r="C534" s="243" t="s">
+        <v>442</v>
+      </c>
+      <c r="D534" s="243" t="s">
         <v>443</v>
-      </c>
-      <c r="D534" s="243" t="s">
-        <v>444</v>
       </c>
       <c r="E534" s="243" t="s">
         <v>22</v>
@@ -14828,10 +14825,10 @@
     </row>
     <row r="535">
       <c r="C535" s="243" t="s">
+        <v>444</v>
+      </c>
+      <c r="D535" s="243" t="s">
         <v>445</v>
-      </c>
-      <c r="D535" s="243" t="s">
-        <v>446</v>
       </c>
       <c r="E535" s="243" t="s">
         <v>22</v>
@@ -14852,10 +14849,10 @@
     </row>
     <row r="536">
       <c r="C536" s="243" t="s">
+        <v>446</v>
+      </c>
+      <c r="D536" s="243" t="s">
         <v>447</v>
-      </c>
-      <c r="D536" s="243" t="s">
-        <v>448</v>
       </c>
       <c r="E536" s="243" t="s">
         <v>22</v>
@@ -14876,10 +14873,10 @@
     </row>
     <row r="537">
       <c r="C537" s="243" t="s">
+        <v>448</v>
+      </c>
+      <c r="D537" s="243" t="s">
         <v>449</v>
-      </c>
-      <c r="D537" s="243" t="s">
-        <v>450</v>
       </c>
       <c r="E537" s="243" t="s">
         <v>22</v>
@@ -14903,7 +14900,7 @@
         <v>81</v>
       </c>
       <c r="D538" s="243" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E538" s="243" t="s">
         <v>22</v>
@@ -14927,7 +14924,7 @@
         <v>84</v>
       </c>
       <c r="D539" s="243" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E539" s="243" t="s">
         <v>22</v>
@@ -14951,7 +14948,7 @@
         <v>36</v>
       </c>
       <c r="D540" s="243" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E540" s="243" t="s">
         <v>22</v>
@@ -14977,7 +14974,7 @@
         <v>39</v>
       </c>
       <c r="D541" s="244" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E541" s="244" t="s">
         <v>22</v>

</xml_diff>